<commit_message>
Add Navigation to do page test case
</commit_message>
<xml_diff>
--- a/QA test cases.xlsx
+++ b/QA test cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ng Hsiao Jiet\ETI-ToDoApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400E6D07-6AE9-47A4-A6A1-F5F6A5BE9A32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712DA82E-A1B0-41C0-AB52-D1E4B7D2FD5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1103" yWindow="1103" windowWidth="18000" windowHeight="9419" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>Test Scenario: To Do App (Navigation and Login)</t>
   </si>
@@ -63,6 +63,18 @@
   </si>
   <si>
     <t>Navigates to To Do page</t>
+  </si>
+  <si>
+    <t>test_&lt;Navigate-To-TpDoPage&gt;</t>
+  </si>
+  <si>
+    <t>This is to test whether user can navigate to To Do page</t>
+  </si>
+  <si>
+    <t>NIL</t>
+  </si>
+  <si>
+    <t>To Do page is shown</t>
   </si>
 </sst>
 </file>
@@ -141,21 +153,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -166,6 +175,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -389,16 +406,16 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A4" sqref="A4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="16"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -429,31 +446,41 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="14">
+      <c r="A3" s="11">
         <v>1</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="14" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="7"/>
+      <c r="A4" s="17">
+        <v>2</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="6"/>
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -492,10 +519,10 @@
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="13"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -538,7 +565,7 @@
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="8"/>
+      <c r="D12" s="7"/>
       <c r="E12" s="4"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
@@ -565,16 +592,16 @@
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="9"/>
+      <c r="D15" s="8"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="13"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -623,8 +650,8 @@
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:7" ht="17.649999999999999" x14ac:dyDescent="0.5">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -641,16 +668,16 @@
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
     </row>
     <row r="23" spans="1:7" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="A23" s="10"/>
+      <c r="A23" s="9"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -662,7 +689,7 @@
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
-      <c r="D24" s="9"/>
+      <c r="D24" s="8"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
@@ -698,7 +725,7 @@
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="11"/>
+      <c r="D28" s="10"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>

</xml_diff>

<commit_message>
Added Navigation to do history page test case
</commit_message>
<xml_diff>
--- a/QA test cases.xlsx
+++ b/QA test cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ng Hsiao Jiet\ETI-ToDoApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712DA82E-A1B0-41C0-AB52-D1E4B7D2FD5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB01542-36BE-4667-AF26-BE2324054E41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1103" yWindow="1103" windowWidth="18000" windowHeight="9419" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
   <si>
     <t>Test Scenario: To Do App (Navigation and Login)</t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>To Do page is shown</t>
+  </si>
+  <si>
+    <t>test_&lt;Navigate-To-ToDoHistoryPage</t>
+  </si>
+  <si>
+    <t>This is to test whether users are able to navigate to To Do History page</t>
+  </si>
+  <si>
+    <t>To Do History page is shown</t>
   </si>
 </sst>
 </file>
@@ -177,14 +186,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,16 +415,16 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:E4"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
+      <c r="B1" s="18"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -465,7 +474,7 @@
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="17">
+      <c r="A4" s="15">
         <v>2</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -477,18 +486,28 @@
       <c r="D4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="16" t="s">
         <v>17</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="A5" s="15">
+        <v>3</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
@@ -519,10 +538,10 @@
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="16"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -598,10 +617,10 @@
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="16"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -650,8 +669,8 @@
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:7" ht="17.649999999999999" x14ac:dyDescent="0.5">
-      <c r="A20" s="15"/>
-      <c r="B20" s="16"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="18"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>

</xml_diff>

<commit_message>
Added Navigation to team contribution page test case
</commit_message>
<xml_diff>
--- a/QA test cases.xlsx
+++ b/QA test cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ng Hsiao Jiet\ETI-ToDoApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB01542-36BE-4667-AF26-BE2324054E41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56BC2EF-0038-44A3-BEF7-EA11C1B1BDD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1103" yWindow="1103" windowWidth="18000" windowHeight="9419" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4485" yWindow="1508" windowWidth="18000" windowHeight="9419" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t>Test Scenario: To Do App (Navigation and Login)</t>
   </si>
@@ -84,6 +84,15 @@
   </si>
   <si>
     <t>To Do History page is shown</t>
+  </si>
+  <si>
+    <t>test_&lt;Navigate-To-TeamContributionsPage&gt;</t>
+  </si>
+  <si>
+    <t>This is to test whether users are able to navigate to Team Contributions page</t>
+  </si>
+  <si>
+    <t>Team contributions page is shown</t>
   </si>
 </sst>
 </file>
@@ -415,7 +424,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -512,11 +521,21 @@
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="A6" s="15">
+        <v>4</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>23</v>
+      </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>

</xml_diff>

<commit_message>
Add Failling login test case
</commit_message>
<xml_diff>
--- a/QA test cases.xlsx
+++ b/QA test cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ng Hsiao Jiet\ETI-ToDoApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56BC2EF-0038-44A3-BEF7-EA11C1B1BDD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2F475F-A614-48ED-9A3C-03E1CBD7B9DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4485" yWindow="1508" windowWidth="18000" windowHeight="9419" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8063" yWindow="2565" windowWidth="18000" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
   <si>
     <t>Test Scenario: To Do App (Navigation and Login)</t>
   </si>
@@ -93,6 +93,21 @@
   </si>
   <si>
     <t>Team contributions page is shown</t>
+  </si>
+  <si>
+    <t>test_&lt;LoginIncorrectUsernameandPassword&gt;</t>
+  </si>
+  <si>
+    <t>This is to test whether user can login with incorrect username or password</t>
+  </si>
+  <si>
+    <t>Error is displayed as such: "You have entered the wrong username/password. Please try again!"</t>
+  </si>
+  <si>
+    <t>username: "username"
+password: "pssword"
+username: "wronguser"
+password: "p@ssw0rd"</t>
   </si>
 </sst>
 </file>
@@ -423,8 +438,8 @@
   </sheetPr>
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -540,10 +555,21 @@
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="A7" s="15">
+        <v>5</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
     </row>

</xml_diff>

<commit_message>
Added pytest test cases for nav and login
</commit_message>
<xml_diff>
--- a/QA test cases.xlsx
+++ b/QA test cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ng Hsiao Jiet\ETI-ToDoApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2F475F-A614-48ED-9A3C-03E1CBD7B9DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2E37A5-C7E6-4B65-AFAB-BC3490642845}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8063" yWindow="2565" windowWidth="18000" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4088" yWindow="1920" windowWidth="18000" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -438,8 +438,8 @@
   </sheetPr>
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Successfully passed 2 nav test cases
</commit_message>
<xml_diff>
--- a/QA test cases.xlsx
+++ b/QA test cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ng Hsiao Jiet\ETI-ToDoApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2E37A5-C7E6-4B65-AFAB-BC3490642845}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB3FFCA-F13D-4125-93DC-7E70617DABB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4088" yWindow="1920" windowWidth="18000" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4763" yWindow="2595" windowWidth="18000" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
   <si>
     <t>Test Scenario: To Do App (Navigation and Login)</t>
   </si>
@@ -108,6 +108,18 @@
 password: "pssword"
 username: "wronguser"
 password: "p@ssw0rd"</t>
+  </si>
+  <si>
+    <t>Don’t have to unit test this page.</t>
+  </si>
+  <si>
+    <t>test_&lt;DisplayListofArchivedItems&gt;</t>
+  </si>
+  <si>
+    <t>This is to test whether users can see a list of archived To Do items in To-Do History page</t>
+  </si>
+  <si>
+    <t>List of archived To Do items displayed</t>
   </si>
 </sst>
 </file>
@@ -143,11 +155,6 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -162,6 +169,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -186,36 +199,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
@@ -438,17 +452,17 @@
   </sheetPr>
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
+      <c r="B1" s="19"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -479,95 +493,101 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="11">
+      <c r="A3" s="10">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="15">
+      <c r="A4" s="14">
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="6"/>
+      <c r="F4" s="16" t="s">
+        <v>17</v>
+      </c>
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="15">
+      <c r="A5" s="14">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" s="17" t="s">
+        <v>20</v>
+      </c>
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="15">
+      <c r="A6" s="14">
         <v>4</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="15" t="s">
         <v>23</v>
       </c>
       <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="G6" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="15">
+      <c r="A7" s="14">
         <v>5</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="15" t="s">
         <v>26</v>
       </c>
       <c r="F7" s="5"/>
@@ -583,10 +603,10 @@
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="18"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -629,7 +649,7 @@
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="7"/>
+      <c r="D12" s="6"/>
       <c r="E12" s="4"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
@@ -656,16 +676,16 @@
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="8"/>
+      <c r="D15" s="7"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="18"/>
+      <c r="B16" s="19"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -696,12 +716,20 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="5"/>
+      <c r="A18" s="14">
+        <v>1</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="17"/>
       <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7" ht="13.15" x14ac:dyDescent="0.4">
@@ -714,8 +742,8 @@
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:7" ht="17.649999999999999" x14ac:dyDescent="0.5">
-      <c r="A20" s="17"/>
-      <c r="B20" s="18"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="19"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -732,16 +760,16 @@
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
     </row>
     <row r="23" spans="1:7" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="A23" s="9"/>
+      <c r="A23" s="8"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -753,7 +781,7 @@
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
-      <c r="D24" s="8"/>
+      <c r="D24" s="7"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
@@ -789,7 +817,7 @@
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="10"/>
+      <c r="D28" s="9"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>

</xml_diff>

<commit_message>
Failed Display archived items test case
</commit_message>
<xml_diff>
--- a/QA test cases.xlsx
+++ b/QA test cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ng Hsiao Jiet\ETI-ToDoApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB3FFCA-F13D-4125-93DC-7E70617DABB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CB3EB0-1787-4C37-9278-30A81C87D11B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4763" yWindow="2595" windowWidth="18000" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
   <si>
     <t>Test Scenario: To Do App (Navigation and Login)</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>List of archived To Do items displayed</t>
+  </si>
+  <si>
+    <t>Failed</t>
   </si>
 </sst>
 </file>
@@ -453,7 +456,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -729,7 +732,9 @@
       <c r="E18" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="17"/>
+      <c r="F18" s="17" t="s">
+        <v>32</v>
+      </c>
       <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7" ht="13.15" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Passed todohist test case
</commit_message>
<xml_diff>
--- a/QA test cases.xlsx
+++ b/QA test cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ng Hsiao Jiet\ETI-ToDoApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CB3EB0-1787-4C37-9278-30A81C87D11B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3563387C-0D45-4DF4-B87A-81199F64753E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4763" yWindow="2595" windowWidth="18000" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1800" yWindow="2363" windowWidth="18000" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
   <si>
     <t>Test Scenario: To Do App (Navigation and Login)</t>
   </si>
@@ -120,9 +120,6 @@
   </si>
   <si>
     <t>List of archived To Do items displayed</t>
-  </si>
-  <si>
-    <t>Failed</t>
   </si>
 </sst>
 </file>
@@ -455,8 +452,8 @@
   </sheetPr>
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -732,8 +729,8 @@
       <c r="E18" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="17" t="s">
-        <v>32</v>
+      <c r="F18" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="G18" s="5"/>
     </row>

</xml_diff>

<commit_message>
Added add blank to-do item test case
</commit_message>
<xml_diff>
--- a/QA test cases.xlsx
+++ b/QA test cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ng Hsiao Jiet\ETI-ToDoApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janinedesiree/github/To-Do_Application/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3563387C-0D45-4DF4-B87A-81199F64753E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E4E782F-8CB4-A347-BE8A-1AC5117B39DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="2363" windowWidth="18000" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9720" yWindow="3040" windowWidth="31020" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
   <si>
     <t>Test Scenario: To Do App (Navigation and Login)</t>
   </si>
@@ -120,6 +120,27 @@
   </si>
   <si>
     <t>List of archived To Do items displayed</t>
+  </si>
+  <si>
+    <t>test_DisplayListOfItems</t>
+  </si>
+  <si>
+    <t>This is to test whether To Do items from any users are shown in a list in the To Do page</t>
+  </si>
+  <si>
+    <t>List of To Do items displayed</t>
+  </si>
+  <si>
+    <t>test_AddBlankItem</t>
+  </si>
+  <si>
+    <t>This is to test whether users are not able to add a To Do Item with no input</t>
+  </si>
+  <si>
+    <t>""</t>
+  </si>
+  <si>
+    <t>No new item is added to list, error message occurs prompting user to enter something in input field</t>
   </si>
 </sst>
 </file>
@@ -206,7 +227,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -232,6 +252,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,24 +473,28 @@
   </sheetPr>
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
+      <c r="B1" s="18"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -492,81 +517,81 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="10">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="9">
         <v>1</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="12" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="14">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="13">
         <v>2</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="15" t="s">
         <v>17</v>
       </c>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="14">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="13">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="16" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="14">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="13">
         <v>4</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="14" t="s">
         <v>23</v>
       </c>
       <c r="F6" s="5"/>
@@ -574,26 +599,26 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="14">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="13">
         <v>5</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="14" t="s">
         <v>26</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -602,18 +627,18 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="18" t="s">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="19"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
@@ -636,25 +661,45 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="5"/>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>1</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="19"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="4"/>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>2</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>38</v>
+      </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -663,7 +708,7 @@
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -672,27 +717,27 @@
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="7"/>
+      <c r="D15" s="6"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="18" t="s">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="19"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>1</v>
       </c>
@@ -715,26 +760,26 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="14">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="13">
         <v>1</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11" t="s">
+      <c r="D18" s="10"/>
+      <c r="E18" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="10" t="s">
         <v>31</v>
       </c>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" ht="14" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -743,16 +788,16 @@
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:7" ht="17.649999999999999" x14ac:dyDescent="0.5">
-      <c r="A20" s="18"/>
-      <c r="B20" s="19"/>
+    <row r="20" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="17"/>
+      <c r="B20" s="18"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -761,17 +806,17 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-    </row>
-    <row r="23" spans="1:7" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="A23" s="8"/>
+    <row r="22" spans="1:7" ht="14" x14ac:dyDescent="0.2">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="1:7" ht="14" x14ac:dyDescent="0.2">
+      <c r="A23" s="7"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -779,16 +824,16 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:7" ht="14" x14ac:dyDescent="0.2">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
-      <c r="D24" s="7"/>
+      <c r="D24" s="6"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="1:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:7" ht="14" x14ac:dyDescent="0.2">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -797,7 +842,7 @@
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -806,7 +851,7 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -815,16 +860,16 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="9"/>
+      <c r="D28" s="8"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>

</xml_diff>

<commit_message>
Added add valid to-do item test case
</commit_message>
<xml_diff>
--- a/QA test cases.xlsx
+++ b/QA test cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janinedesiree/github/To-Do_Application/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E4E782F-8CB4-A347-BE8A-1AC5117B39DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFB394A-620B-CD43-8056-74FEE83A3DDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9720" yWindow="3040" windowWidth="31020" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
   <si>
     <t>Test Scenario: To Do App (Navigation and Login)</t>
   </si>
@@ -141,6 +141,18 @@
   </si>
   <si>
     <t>No new item is added to list, error message occurs prompting user to enter something in input field</t>
+  </si>
+  <si>
+    <t>test_AddValidItem</t>
+  </si>
+  <si>
+    <t>This is to test whether users can add a To Do Item with valid parameters</t>
+  </si>
+  <si>
+    <t>"jd's test item"</t>
+  </si>
+  <si>
+    <t>Item is added to the list</t>
   </si>
 </sst>
 </file>
@@ -474,7 +486,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -700,11 +712,21 @@
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="A13" s="4">
+        <v>3</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>

</xml_diff>

<commit_message>
Added add existing to-do item test case
</commit_message>
<xml_diff>
--- a/QA test cases.xlsx
+++ b/QA test cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janinedesiree/github/To-Do_Application/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFB394A-620B-CD43-8056-74FEE83A3DDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5125415D-D606-2948-984E-401D79B9B83B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9720" yWindow="3040" windowWidth="31020" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14160" yWindow="3040" windowWidth="31020" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>Test Scenario: To Do App (Navigation and Login)</t>
   </si>
@@ -134,9 +134,6 @@
     <t>test_AddBlankItem</t>
   </si>
   <si>
-    <t>This is to test whether users are not able to add a To Do Item with no input</t>
-  </si>
-  <si>
     <t>""</t>
   </si>
   <si>
@@ -146,13 +143,22 @@
     <t>test_AddValidItem</t>
   </si>
   <si>
-    <t>This is to test whether users can add a To Do Item with valid parameters</t>
-  </si>
-  <si>
     <t>"jd's test item"</t>
   </si>
   <si>
     <t>Item is added to the list</t>
+  </si>
+  <si>
+    <t>test_AddExistingItem</t>
+  </si>
+  <si>
+    <t>This is to test that users can add a To Do item that already exists</t>
+  </si>
+  <si>
+    <t>This is to test that users can add a To Do Item with valid parameters</t>
+  </si>
+  <si>
+    <t>This is to test that users are not able to add a To Do Item with no input</t>
   </si>
 </sst>
 </file>
@@ -232,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -262,6 +268,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -486,7 +493,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -496,10 +503,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
+      <c r="B1" s="19"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -640,10 +647,10 @@
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="18"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -683,30 +690,30 @@
       <c r="C11" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="19"/>
+      <c r="F11" s="20"/>
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>2</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="E12" s="20" t="s">
         <v>37</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>38</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
@@ -715,27 +722,35 @@
       <c r="A13" s="4">
         <v>3</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="E13" s="20" t="s">
         <v>40</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>42</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
+      <c r="A14" s="17">
+        <v>4</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+      <c r="E14" s="20" t="s">
+        <v>40</v>
+      </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
@@ -749,10 +764,10 @@
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="18"/>
+      <c r="B16" s="19"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -811,8 +826,8 @@
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A20" s="17"/>
-      <c r="B20" s="18"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="19"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>

</xml_diff>

<commit_message>
Added delete items from to-do list test case
</commit_message>
<xml_diff>
--- a/QA test cases.xlsx
+++ b/QA test cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janinedesiree/github/To-Do_Application/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5125415D-D606-2948-984E-401D79B9B83B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A6E1A7-EC72-0A48-A9CC-922BA4D5381A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14160" yWindow="3040" windowWidth="31020" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13620" yWindow="2700" windowWidth="31020" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
   <si>
     <t>Test Scenario: To Do App (Navigation and Login)</t>
   </si>
@@ -159,6 +159,15 @@
   </si>
   <si>
     <t>This is to test that users are not able to add a To Do Item with no input</t>
+  </si>
+  <si>
+    <t>test_DeleteItem</t>
+  </si>
+  <si>
+    <t>This is to test that users can delete items in To-Do list</t>
+  </si>
+  <si>
+    <t>Item is deleted successfully</t>
   </si>
 </sst>
 </file>
@@ -490,10 +499,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -754,118 +763,128 @@
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+    <row r="15" spans="1:7" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="17">
+        <v>5</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="B17" s="19"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="13">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="13">
         <v>1</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B19" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C19" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10" t="s">
+      <c r="D19" s="10"/>
+      <c r="E19" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F19" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A20" s="18"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
+    <row r="20" spans="1:7" ht="14" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A21" s="18"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" ht="14" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
+      <c r="A24" s="7"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
-      <c r="D24" s="6"/>
+      <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
@@ -874,19 +893,19 @@
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+      <c r="D25" s="6"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+    <row r="26" spans="1:7" ht="14" x14ac:dyDescent="0.2">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
     </row>
     <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
@@ -901,7 +920,7 @@
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="8"/>
+      <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -910,17 +929,26 @@
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
+      <c r="D29" s="8"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A21:B21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Added logout test case
</commit_message>
<xml_diff>
--- a/QA test cases.xlsx
+++ b/QA test cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janinedesiree/github/To-Do_Application/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A6E1A7-EC72-0A48-A9CC-922BA4D5381A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4927BB9B-1D84-5747-A1EB-D83127F3B670}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13620" yWindow="2700" windowWidth="31020" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2900" yWindow="680" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="52">
   <si>
     <t>Test Scenario: To Do App (Navigation and Login)</t>
   </si>
@@ -68,9 +68,6 @@
     <t>test_&lt;Navigate-To-TpDoPage&gt;</t>
   </si>
   <si>
-    <t>This is to test whether user can navigate to To Do page</t>
-  </si>
-  <si>
     <t>NIL</t>
   </si>
   <si>
@@ -80,36 +77,18 @@
     <t>test_&lt;Navigate-To-ToDoHistoryPage</t>
   </si>
   <si>
-    <t>This is to test whether users are able to navigate to To Do History page</t>
-  </si>
-  <si>
     <t>To Do History page is shown</t>
   </si>
   <si>
     <t>test_&lt;Navigate-To-TeamContributionsPage&gt;</t>
   </si>
   <si>
-    <t>This is to test whether users are able to navigate to Team Contributions page</t>
-  </si>
-  <si>
     <t>Team contributions page is shown</t>
   </si>
   <si>
-    <t>test_&lt;LoginIncorrectUsernameandPassword&gt;</t>
-  </si>
-  <si>
     <t>This is to test whether user can login with incorrect username or password</t>
   </si>
   <si>
-    <t>Error is displayed as such: "You have entered the wrong username/password. Please try again!"</t>
-  </si>
-  <si>
-    <t>username: "username"
-password: "pssword"
-username: "wronguser"
-password: "p@ssw0rd"</t>
-  </si>
-  <si>
     <t>Don’t have to unit test this page.</t>
   </si>
   <si>
@@ -168,6 +147,38 @@
   </si>
   <si>
     <t>Item is deleted successfully</t>
+  </si>
+  <si>
+    <t>This is to test whether users are able to navigate to To Do History page after logging in</t>
+  </si>
+  <si>
+    <t>This is to test whether users are able to navigate to Team Contributions page logging in</t>
+  </si>
+  <si>
+    <t>This is to test whether user can navigate to To Do page after page logging in</t>
+  </si>
+  <si>
+    <t>test_&lt;InvalidLogin&gt;</t>
+  </si>
+  <si>
+    <t>username: "myusername"
+password: "mypassword"</t>
+  </si>
+  <si>
+    <t>username: "wrongusername"
+password: "wrongpassword"</t>
+  </si>
+  <si>
+    <t>Error is displayed as such: "Incorrect username and password. Please try again."</t>
+  </si>
+  <si>
+    <t>test_&lt;test_Logout&gt;</t>
+  </si>
+  <si>
+    <t>This is to test that users can logout</t>
+  </si>
+  <si>
+    <t>Message saying "Logged out" is shown</t>
   </si>
 </sst>
 </file>
@@ -247,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -266,21 +277,46 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,16 +535,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="72.6640625" customWidth="1"/>
+    <col min="4" max="4" width="25.5" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="26"/>
+    <col min="6" max="6" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -518,7 +557,7 @@
       <c r="B1" s="19"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="E1" s="22"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
@@ -535,7 +574,7 @@
       <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="22" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -558,379 +597,389 @@
       <c r="D3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="23" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="13">
+      <c r="A4" s="12">
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="E4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="F4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="12">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13">
-        <v>3</v>
-      </c>
-      <c r="B5" s="10" t="s">
+      <c r="C5" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="F5" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12">
+        <v>4</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="14" t="s">
+      <c r="C6" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="24" t="s">
         <v>20</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="13">
-        <v>4</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>23</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="13">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="16" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="20">
         <v>5</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>25</v>
+      <c r="B7" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>21</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:7" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="20"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="29"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:7" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="12">
+        <v>6</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="B11" s="19"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E12" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
-        <v>1</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
-        <v>2</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
-        <v>3</v>
-      </c>
-      <c r="B13" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>2</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="17">
-        <v>4</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="20" t="s">
-        <v>40</v>
+      <c r="D14" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="17">
-        <v>5</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>46</v>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <v>3</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>37</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+        <v>33</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="5"/>
+      <c r="A16" s="15">
+        <v>4</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="10" t="s">
+        <v>34</v>
+      </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="15">
+        <v>5</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="B19" s="19"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E20" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F20" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G20" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="13">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="12">
         <v>1</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-    </row>
-    <row r="21" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A21" s="18"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-    </row>
-    <row r="24" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A24" s="7"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
+      <c r="B21" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:7" ht="14" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A23" s="18"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A26" s="5"/>
+      <c r="A26" s="7"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
+      <c r="E26" s="25"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+    <row r="27" spans="1:7" ht="14" x14ac:dyDescent="0.2">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="1:7" ht="14" x14ac:dyDescent="0.2">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
     </row>
     <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="28"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
     </row>
@@ -939,16 +988,38 @@
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
+      <c r="E30" s="28"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
     </row>
+    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
+    <mergeCell ref="E7:E8"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Added failing navigation to ToDo page test case
</commit_message>
<xml_diff>
--- a/QA test cases.xlsx
+++ b/QA test cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janinedesiree/github/To-Do_Application/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4927BB9B-1D84-5747-A1EB-D83127F3B670}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC983FD-038D-5249-A59A-A631A656F39F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2900" yWindow="680" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
   <si>
     <t>Test Scenario: To Do App (Navigation and Login)</t>
   </si>
@@ -172,6 +172,12 @@
     <t>Error is displayed as such: "Incorrect username and password. Please try again."</t>
   </si>
   <si>
+    <t>test_&lt;test_CannotNavigateToDoPage&gt;</t>
+  </si>
+  <si>
+    <t>This is to test that users cannot navigate to To Do page without logging in</t>
+  </si>
+  <si>
     <t>test_&lt;test_Logout&gt;</t>
   </si>
   <si>
@@ -179,6 +185,9 @@
   </si>
   <si>
     <t>Message saying "Logged out" is shown</t>
+  </si>
+  <si>
+    <t>Error message saying "Please login to see this page." is shown</t>
   </si>
 </sst>
 </file>
@@ -535,10 +544,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -701,266 +710,276 @@
         <v>6</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="10"/>
+        <v>52</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="E9" s="24" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="25"/>
+      <c r="A10" s="16">
+        <v>6</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>54</v>
+      </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="18" t="s">
+    <row r="11" spans="1:7" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="B12" s="19"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E13" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G13" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4">
-        <v>1</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
-        <v>2</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>38</v>
+        <v>1</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F14" s="17"/>
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="15">
-        <v>4</v>
+      <c r="A16" s="4">
+        <v>3</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="4"/>
+        <v>37</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>33</v>
+      </c>
       <c r="E16" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="15">
+        <v>4</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="15">
         <v>5</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B18" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C18" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D18" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="26" t="s">
+      <c r="E18" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="18" t="s">
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19" spans="1:7" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="B20" s="19"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B21" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="22" t="s">
+      <c r="E21" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G21" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="12">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="12">
         <v>1</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B22" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C22" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10" t="s">
+      <c r="D22" s="10"/>
+      <c r="E22" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F22" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="G21" s="5"/>
-    </row>
-    <row r="22" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="5"/>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A23" s="18"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
+    <row r="23" spans="1:7" ht="14" x14ac:dyDescent="0.2">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A24" s="18"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
       <c r="E24" s="22"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" ht="14" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A27" s="5"/>
+      <c r="A27" s="7"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
-      <c r="D27" s="6"/>
+      <c r="D27" s="5"/>
       <c r="E27" s="25"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
@@ -969,19 +988,19 @@
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+      <c r="D28" s="6"/>
       <c r="E28" s="25"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
+    <row r="29" spans="1:7" ht="14" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
@@ -996,7 +1015,7 @@
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="8"/>
+      <c r="D31" s="2"/>
       <c r="E31" s="28"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
@@ -1005,18 +1024,27 @@
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+      <c r="D32" s="8"/>
       <c r="E32" s="28"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A24:B24"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="A7:A8"/>

</xml_diff>

<commit_message>
Added failing navigation to To Do History test case
</commit_message>
<xml_diff>
--- a/QA test cases.xlsx
+++ b/QA test cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janinedesiree/github/To-Do_Application/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC983FD-038D-5249-A59A-A631A656F39F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7688D4-8170-FC41-A4B5-B923A5A6FA7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2900" yWindow="680" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
   <si>
     <t>Test Scenario: To Do App (Navigation and Login)</t>
   </si>
@@ -172,15 +172,9 @@
     <t>Error is displayed as such: "Incorrect username and password. Please try again."</t>
   </si>
   <si>
-    <t>test_&lt;test_CannotNavigateToDoPage&gt;</t>
-  </si>
-  <si>
     <t>This is to test that users cannot navigate to To Do page without logging in</t>
   </si>
   <si>
-    <t>test_&lt;test_Logout&gt;</t>
-  </si>
-  <si>
     <t>This is to test that users can logout</t>
   </si>
   <si>
@@ -188,6 +182,18 @@
   </si>
   <si>
     <t>Error message saying "Please login to see this page." is shown</t>
+  </si>
+  <si>
+    <t>test_&lt;CannotNavigateToDoPage&gt;</t>
+  </si>
+  <si>
+    <t>test_&lt;Logout&gt;</t>
+  </si>
+  <si>
+    <t>test_&lt;CannotNavigateToDoHistory&gt;</t>
+  </si>
+  <si>
+    <t>This is to test that users cannot navigate to To Do History page without logging in</t>
   </si>
 </sst>
 </file>
@@ -544,10 +550,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -710,285 +716,295 @@
         <v>6</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="16">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B10" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>49</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>50</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="11"/>
+      <c r="A11" s="12">
+        <v>8</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>52</v>
+      </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
+    <row r="12" spans="1:7" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="B13" s="19"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E14" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4">
-        <v>1</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="17"/>
-      <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
-        <v>2</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>38</v>
+        <v>1</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F15" s="17"/>
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="15">
-        <v>4</v>
+      <c r="A17" s="4">
+        <v>3</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="4"/>
+        <v>37</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>33</v>
+      </c>
       <c r="E17" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="1:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15">
+        <v>4</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="15">
         <v>5</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B19" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C19" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D19" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="26" t="s">
+      <c r="E19" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="1:7" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="25"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="18" t="s">
+    <row r="20" spans="1:7" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="B21" s="19"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="22" t="s">
+      <c r="E22" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G22" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="12">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="12">
         <v>1</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B23" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C23" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10" t="s">
+      <c r="D23" s="10"/>
+      <c r="E23" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F23" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A24" s="18"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
+    <row r="24" spans="1:7" ht="14" x14ac:dyDescent="0.2">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A25" s="18"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
       <c r="E25" s="22"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:7" ht="14" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A28" s="5"/>
+      <c r="A28" s="7"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
-      <c r="D28" s="6"/>
+      <c r="D28" s="5"/>
       <c r="E28" s="25"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -997,19 +1013,19 @@
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
+      <c r="D29" s="6"/>
       <c r="E29" s="25"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
     </row>
-    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
+    <row r="30" spans="1:7" ht="14" x14ac:dyDescent="0.2">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
     </row>
     <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
@@ -1024,7 +1040,7 @@
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="8"/>
+      <c r="D32" s="2"/>
       <c r="E32" s="28"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
@@ -1033,18 +1049,27 @@
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
+      <c r="D33" s="8"/>
       <c r="E33" s="28"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A25:B25"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="A7:A8"/>

</xml_diff>

<commit_message>
Did final run of all tests and passed
</commit_message>
<xml_diff>
--- a/QA test cases.xlsx
+++ b/QA test cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janinedesiree/github/To-Do_Application/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7688D4-8170-FC41-A4B5-B923A5A6FA7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B4CB28-1BF3-8A48-A8AB-BE95DE66A819}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2900" yWindow="680" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="64">
   <si>
     <t>Test Scenario: To Do App (Navigation and Login)</t>
   </si>
@@ -194,6 +194,27 @@
   </si>
   <si>
     <t>This is to test that users cannot navigate to To Do History page without logging in</t>
+  </si>
+  <si>
+    <t>Displayed</t>
+  </si>
+  <si>
+    <t>Item not added, error message shown</t>
+  </si>
+  <si>
+    <t>Item added</t>
+  </si>
+  <si>
+    <t>Item deleted and removed from list</t>
+  </si>
+  <si>
+    <t>User cannot login, error message displayed</t>
+  </si>
+  <si>
+    <t>User can log out, message displayed</t>
+  </si>
+  <si>
+    <t>user cannot navigate, error message displayed</t>
   </si>
 </sst>
 </file>
@@ -300,37 +321,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -553,7 +574,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -561,18 +582,18 @@
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="72.6640625" customWidth="1"/>
     <col min="4" max="4" width="25.5" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" style="26"/>
+    <col min="5" max="5" width="14.33203125" style="22"/>
     <col min="6" max="6" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
+      <c r="B1" s="27"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="22"/>
+      <c r="E1" s="18"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
@@ -589,7 +610,7 @@
       <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="18" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -612,7 +633,7 @@
       <c r="D3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="19" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="5"/>
@@ -631,7 +652,7 @@
       <c r="D4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="20" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="13" t="s">
@@ -652,7 +673,7 @@
       <c r="D5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F5" s="14" t="s">
@@ -673,7 +694,7 @@
       <c r="D6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="20" t="s">
         <v>20</v>
       </c>
       <c r="F6" s="5"/>
@@ -682,33 +703,37 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="16" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="20">
+      <c r="A7" s="29">
         <v>5</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="28" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="6"/>
+      <c r="F7" s="14" t="s">
+        <v>61</v>
+      </c>
       <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="20"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
       <c r="D8" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="29"/>
-      <c r="F8" s="6"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="14" t="s">
+        <v>61</v>
+      </c>
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -724,10 +749,12 @@
       <c r="D9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="6"/>
+      <c r="F9" s="14" t="s">
+        <v>62</v>
+      </c>
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -746,7 +773,9 @@
       <c r="E10" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="14" t="s">
+        <v>63</v>
+      </c>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -765,7 +794,9 @@
       <c r="E11" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="6"/>
+      <c r="F11" s="14" t="s">
+        <v>63</v>
+      </c>
       <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:7" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -777,13 +808,13 @@
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="19"/>
+      <c r="B13" s="27"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="22"/>
+      <c r="E13" s="18"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
@@ -800,7 +831,7 @@
       <c r="D14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E14" s="18" t="s">
         <v>5</v>
       </c>
       <c r="F14" s="3" t="s">
@@ -826,7 +857,9 @@
       <c r="E15" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="17"/>
+      <c r="F15" s="14" t="s">
+        <v>57</v>
+      </c>
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -845,7 +878,9 @@
       <c r="E16" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="5"/>
+      <c r="F16" s="14" t="s">
+        <v>58</v>
+      </c>
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -864,7 +899,9 @@
       <c r="E17" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F17" s="5"/>
+      <c r="F17" s="14" t="s">
+        <v>59</v>
+      </c>
       <c r="G17" s="5"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -881,7 +918,9 @@
       <c r="E18" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="5"/>
+      <c r="F18" s="14" t="s">
+        <v>59</v>
+      </c>
       <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -897,28 +936,30 @@
       <c r="D19" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="26" t="s">
+      <c r="E19" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="6"/>
+      <c r="F19" s="14" t="s">
+        <v>60</v>
+      </c>
       <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="25"/>
+      <c r="E20" s="21"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="19"/>
+      <c r="B21" s="27"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="22"/>
+      <c r="E21" s="18"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
@@ -935,7 +976,7 @@
       <c r="D22" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="22" t="s">
+      <c r="E22" s="18" t="s">
         <v>5</v>
       </c>
       <c r="F22" s="3" t="s">
@@ -969,16 +1010,16 @@
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="25"/>
+      <c r="E24" s="21"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
     </row>
     <row r="25" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A25" s="18"/>
-      <c r="B25" s="19"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="27"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="22"/>
+      <c r="E25" s="18"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
@@ -987,7 +1028,7 @@
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="22"/>
+      <c r="E26" s="18"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
@@ -996,7 +1037,7 @@
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
-      <c r="E27" s="27"/>
+      <c r="E27" s="23"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
     </row>
@@ -1005,7 +1046,7 @@
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
-      <c r="E28" s="25"/>
+      <c r="E28" s="21"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
     </row>
@@ -1014,7 +1055,7 @@
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="6"/>
-      <c r="E29" s="25"/>
+      <c r="E29" s="21"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
     </row>
@@ -1023,7 +1064,7 @@
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="25"/>
+      <c r="E30" s="21"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
     </row>
@@ -1032,7 +1073,7 @@
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
-      <c r="E31" s="28"/>
+      <c r="E31" s="24"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
@@ -1041,7 +1082,7 @@
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="28"/>
+      <c r="E32" s="24"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
     </row>
@@ -1050,7 +1091,7 @@
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="8"/>
-      <c r="E33" s="28"/>
+      <c r="E33" s="24"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
     </row>
@@ -1059,7 +1100,7 @@
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="28"/>
+      <c r="E34" s="24"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
     </row>

</xml_diff>